<commit_message>
New 32 region classification. First runs with a selection of data feeds show a very good process balance.
</commit_message>
<xml_diff>
--- a/Settings/Base/040_BaseRegionClassification.xlsx
+++ b/Settings/Base/040_BaseRegionClassification.xlsx
@@ -346,7 +346,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,7 +362,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -629,9 +629,11 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>